<commit_message>
added prokka to workflow
</commit_message>
<xml_diff>
--- a/input_instructions/pipevar_defaults.xlsx
+++ b/input_instructions/pipevar_defaults.xlsx
@@ -31,12 +31,6 @@
     <t xml:space="preserve">startOver</t>
   </si>
   <si>
-    <t xml:space="preserve">isPreprocess_fastq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keep_LocusName</t>
-  </si>
-  <si>
     <t xml:space="preserve">server</t>
   </si>
   <si>
@@ -214,6 +208,9 @@
     <t xml:space="preserve">recreate_reports</t>
   </si>
   <si>
+    <t xml:space="preserve">assembly_folder</t>
+  </si>
+  <si>
     <t xml:space="preserve">n</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">same_strain_isolates.mat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/kishonylab/KishonyStorage/noga/MaccabiUTI/Mathews_processing/Filtered_data/</t>
   </si>
 </sst>
 </file>
@@ -352,12 +352,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -367,57 +367,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL2"/>
+  <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BL3" activeCellId="0" sqref="BL3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="26" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="38.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="28.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="14.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="52" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="24" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="38.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="29.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="28.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,22 +543,22 @@
       <c r="AP1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="AR1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="AU1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="0" t="s">
         <v>47</v>
       </c>
       <c r="AW1" s="0" t="s">
@@ -609,9 +605,6 @@
       </c>
       <c r="BK1" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="BL1" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,184 +621,181 @@
         <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="O2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>10000</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="O2" s="0" t="n">
+      <c r="Q2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="P2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="T2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="W2" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="X2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="0" t="s">
+      <c r="AF2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AH2" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="Z2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="AD2" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AE2" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AF2" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="AG2" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="AH2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
+      <c r="AI2" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="AK2" s="0" t="s">
+      <c r="AJ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="AL2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AO2" s="0" t="n">
-        <v>1</v>
+      <c r="AO2" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ2" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="AR2" s="0" t="s">
+      <c r="AQ2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AR2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="AS2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AT2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX2" s="0" t="n">
-        <v>5</v>
+      <c r="AX2" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BA2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BB2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BC2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="BE2" s="0" t="s">
+      <c r="BD2" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BE2" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BF2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="BG2" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="BH2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="BI2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="BF2" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BG2" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BH2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI2" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="BJ2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="BK2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL2" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
just a commit before the delete
</commit_message>
<xml_diff>
--- a/input_instructions/pipevar_defaults.xlsx
+++ b/input_instructions/pipevar_defaults.xlsx
@@ -31,12 +31,6 @@
     <t xml:space="preserve">startOver</t>
   </si>
   <si>
-    <t xml:space="preserve">isPreprocess_fastq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">keep_LocusName</t>
-  </si>
-  <si>
     <t xml:space="preserve">server</t>
   </si>
   <si>
@@ -214,6 +208,9 @@
     <t xml:space="preserve">recreate_reports</t>
   </si>
   <si>
+    <t xml:space="preserve">assembly_folder</t>
+  </si>
+  <si>
     <t xml:space="preserve">n</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">same_strain_isolates.mat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/media/kishonylab/KishonyStorage/noga/MaccabiUTI/Mathews_processing/Filtered_data/</t>
   </si>
 </sst>
 </file>
@@ -352,12 +352,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -367,57 +367,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL2"/>
+  <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AT1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BL3" activeCellId="0" sqref="BL3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.3828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="26" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="38.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="28.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="14.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="52" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="24" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="38.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="29.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="28.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="14.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="12.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,22 +543,22 @@
       <c r="AP1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="0" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="AR1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="0" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
       <c r="AU1" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="0" t="s">
         <v>47</v>
       </c>
       <c r="AW1" s="0" t="s">
@@ -609,9 +605,6 @@
       </c>
       <c r="BK1" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="BL1" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,184 +621,181 @@
         <v>1</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="N2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="O2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="M2" s="0" t="n">
-        <v>10000</v>
-      </c>
-      <c r="N2" s="0" t="n">
-        <v>300</v>
-      </c>
-      <c r="O2" s="0" t="n">
+      <c r="Q2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="V2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AC2" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AD2" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="P2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="T2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="V2" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="W2" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="X2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="0" t="s">
+      <c r="AF2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="AH2" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="Z2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="AD2" s="0" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AE2" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AF2" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="AG2" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="AH2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI2" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
+      <c r="AI2" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="AK2" s="0" t="s">
+      <c r="AJ2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="AL2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN2" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="AO2" s="0" t="n">
-        <v>1</v>
+      <c r="AO2" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ2" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="AR2" s="0" t="s">
+      <c r="AQ2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AR2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="AS2" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="AT2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX2" s="0" t="n">
-        <v>5</v>
+      <c r="AX2" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BA2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BB2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="BC2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="BD2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="BE2" s="0" t="s">
+      <c r="BD2" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BE2" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="BF2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="BG2" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="BH2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="BI2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK2" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="BF2" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BG2" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="BH2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI2" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="BJ2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="BK2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL2" s="0" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>